<commit_message>
Revert broken OptimizedExcelWriter class to fix Excel output
The OptimizedExcelWriter class introduced in the excel_writer_optimizations
commit was causing broken Excel files. The issue was the 'constant_memory': True
option in xlsxwriter, which prevents modifying cells after they're written.

This caused incomplete data writing where only the first column was populated
and all other columns were missing from the output sheets.

Changes:
- Removed the entire OptimizedExcelWriter class
- Restored the working apply_excel_formatting function from api_call_optimizations
- Reverted Excel generation to use pd.ExcelWriter directly
- Output now matches the working api_call_optimizations commit (37KB with full data)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/CJA_DataView_Adobe Store - Prod CJA Lab L123 Adobe Summit 2025_dv_677ea9291244fd082f02dd42_SDR.xlsx
+++ b/CJA_DataView_Adobe Store - Prod CJA Lab L123 Adobe Summit 2025_dv_677ea9291244fd082f02dd42_SDR.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2275" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2275" uniqueCount="779">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Data Quality Summary</t>
   </si>
   <si>
-    <t>2026-01-06 10:34:03 PST</t>
+    <t>2026-01-07 12:01:20 PST</t>
   </si>
   <si>
     <t>dv_677ea9291244fd082f02dd42</t>
@@ -615,7 +615,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "metrics/visitors",
-  "relevancyScore": 0.021276597,
+  "relevancyScore": 0.021739129,
   "companyCount": 5
 }</t>
   </si>
@@ -624,7 +624,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "metrics/visits",
-  "relevancyScore": 0.012765957,
+  "relevancyScore": 0.013043478,
   "companyCount": 3
 }</t>
   </si>
@@ -633,7 +633,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "metrics/order_quantity",
-  "relevancyScore": 0.004255319,
+  "relevancyScore": 0.0043478264,
   "companyCount": 1
 }</t>
   </si>
@@ -642,7 +642,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "metrics/orders_1",
-  "relevancyScore": 0.004255319,
+  "relevancyScore": 0.0043478264,
   "companyCount": 1
 }</t>
   </si>
@@ -651,7 +651,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "metrics/orders",
-  "relevancyScore": 0.021276597,
+  "relevancyScore": 0.021739129,
   "companyCount": 5
 }</t>
   </si>
@@ -660,7 +660,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "metrics/commerce.purchases.value",
-  "relevancyScore": 0.021276597,
+  "relevancyScore": 0.021739129,
   "companyCount": 5
 }</t>
   </si>
@@ -669,8 +669,8 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "metrics/occurrences",
-  "relevancyScore": 0.114893615,
-  "companyCount": 27
+  "relevancyScore": 0.11304347,
+  "companyCount": 26
 }</t>
   </si>
   <si>
@@ -2234,7 +2234,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/daterangesecond",
-  "relevancyScore": 0.001923077,
+  "relevancyScore": 0.001980198,
   "companyCount": 1
 }</t>
   </si>
@@ -2243,7 +2243,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/66577f485e767a2c9e40b94d._experience.decisioning.propositions.scopeDetails.correlationID.activityName",
-  "relevancyScore": 0.001923077,
+  "relevancyScore": 0.001980198,
   "companyCount": 1
 }</t>
   </si>
@@ -2252,7 +2252,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/adobe_timespentpersession",
-  "relevancyScore": 0.001923077,
+  "relevancyScore": 0.001980198,
   "companyCount": 1
 }</t>
   </si>
@@ -2261,8 +2261,8 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/platformdatasetid",
-  "relevancyScore": 0.003846154,
-  "companyCount": 2
+  "relevancyScore": 0.0059405942,
+  "companyCount": 3
 }</t>
   </si>
   <si>
@@ -2270,7 +2270,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/timepartdayofweek",
-  "relevancyScore": 0.005769231,
+  "relevancyScore": 0.0059405942,
   "companyCount": 3
 }</t>
   </si>
@@ -2279,7 +2279,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/session_referrer",
-  "relevancyScore": 0.001923077,
+  "relevancyScore": 0.001980198,
   "companyCount": 1
 }</t>
   </si>
@@ -2288,17 +2288,8 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/page_name",
-  "relevancyScore": 0.028846154,
+  "relevancyScore": 0.02970297,
   "companyCount": 15
-}</t>
-  </si>
-  <si>
-    <t>{
-  "count": 0,
-  "mostRecentTimestamp": null,
-  "itemId": "variables/timepartmonthofyear",
-  "relevancyScore": 0.001923077,
-  "companyCount": 1
 }</t>
   </si>
   <si>
@@ -2306,7 +2297,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/adobe_personid",
-  "relevancyScore": 0.007692308,
+  "relevancyScore": 0.007920792,
   "companyCount": 4
 }</t>
   </si>
@@ -2315,7 +2306,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/daterangehour",
-  "relevancyScore": 0.021153847,
+  "relevancyScore": 0.021782178,
   "companyCount": 11
 }</t>
   </si>
@@ -2324,8 +2315,8 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/daterangemonth",
-  "relevancyScore": 0.007692308,
-  "companyCount": 4
+  "relevancyScore": 0.0059405942,
+  "companyCount": 3
 }</t>
   </si>
   <si>
@@ -2333,7 +2324,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/product_name",
-  "relevancyScore": 0.015384616,
+  "relevancyScore": 0.015841585,
   "companyCount": 8
 }</t>
   </si>
@@ -2342,7 +2333,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/daterangeday",
-  "relevancyScore": 0.015384616,
+  "relevancyScore": 0.015841585,
   "companyCount": 8
 }</t>
   </si>
@@ -2351,7 +2342,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/event_type",
-  "relevancyScore": 0.005769231,
+  "relevancyScore": 0.0059405942,
   "companyCount": 3
 }</t>
   </si>
@@ -2360,7 +2351,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/state_province",
-  "relevancyScore": 0.003846154,
+  "relevancyScore": 0.003960396,
   "companyCount": 2
 }</t>
   </si>
@@ -2369,7 +2360,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/directMarketing.hashedEmail",
-  "relevancyScore": 0.025,
+  "relevancyScore": 0.025742576,
   "companyCount": 13
 }</t>
   </si>
@@ -2378,7 +2369,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/environment.browserDetails._acxpevangelist.customUserAgent",
-  "relevancyScore": 0.003846154,
+  "relevancyScore": 0.003960396,
   "companyCount": 2
 }</t>
   </si>
@@ -2387,8 +2378,8 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/adobe_identitynamespace",
-  "relevancyScore": 0.034615386,
-  "companyCount": 18
+  "relevancyScore": 0.03168317,
+  "companyCount": 16
 }</t>
   </si>
   <si>
@@ -2396,7 +2387,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/66577f485e767a2c9e40b94d._experience.decisioning.propositions.scopeDetails.correlationID.experienceName",
-  "relevancyScore": 0.001923077,
+  "relevancyScore": 0.001980198,
   "companyCount": 1
 }</t>
   </si>
@@ -2405,7 +2396,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/browser_name",
-  "relevancyScore": 0.001923077,
+  "relevancyScore": 0.001980198,
   "companyCount": 1
 }</t>
   </si>
@@ -2414,7 +2405,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/pages_and_actions",
-  "relevancyScore": 0.003846154,
+  "relevancyScore": 0.003960396,
   "companyCount": 2
 }</t>
   </si>
@@ -2423,7 +2414,7 @@
   "count": 0,
   "mostRecentTimestamp": null,
   "itemId": "variables/referring_url",
-  "relevancyScore": 0.003846154,
+  "relevancyScore": 0.003960396,
   "companyCount": 2
 }</t>
   </si>
@@ -9480,13 +9471,13 @@
         <v>0</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="Q2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S2" s="2" t="b">
         <v>1</v>
@@ -9533,10 +9524,10 @@
         <v>0</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S3" s="3" t="b">
         <v>0</v>
@@ -9616,19 +9607,19 @@
         <v>0</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S4" s="2" t="b">
         <v>0</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="Y4" s="2" t="s">
         <v>228</v>
@@ -9690,40 +9681,40 @@
         <v>0</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="V5" s="3" t="s">
         <v>382</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="Y5" s="3" t="s">
         <v>228</v>
       </c>
       <c r="Z5" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="AA5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="3" t="s">
         <v>748</v>
-      </c>
-      <c r="AA5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="3" t="s">
-        <v>749</v>
       </c>
       <c r="AC5" s="3" t="b">
         <v>1</v>
@@ -9732,10 +9723,10 @@
         <v>240</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="AF5" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="6" spans="1:33" s="2" customFormat="1" ht="105" customHeight="1">
@@ -9782,7 +9773,7 @@
         <v>0</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="S6" s="2" t="b">
         <v>1</v>
@@ -9832,40 +9823,40 @@
         <v>0</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S7" s="3" t="b">
         <v>0</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="V7" s="3" t="s">
         <v>384</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="Y7" s="3" t="s">
         <v>228</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AA7" s="3" t="b">
         <v>0</v>
       </c>
       <c r="AB7" s="3" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="AC7" s="3" t="b">
         <v>1</v>
@@ -9921,13 +9912,13 @@
         <v>0</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="Q8" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S8" s="2" t="b">
         <v>0</v>
@@ -9977,25 +9968,25 @@
         <v>0</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S9" s="3" t="b">
         <v>0</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="X9" s="3" t="s">
         <v>266</v>
@@ -10010,7 +10001,7 @@
         <v>0</v>
       </c>
       <c r="AB9" s="3" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="AC9" s="3" t="b">
         <v>0</v>
@@ -10066,13 +10057,13 @@
         <v>0</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="Q10" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S10" s="2" t="b">
         <v>0</v>
@@ -10131,13 +10122,13 @@
         <v>0</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="Q11" s="3" t="b">
         <v>1</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S11" s="3" t="b">
         <v>0</v>
@@ -10181,10 +10172,10 @@
         <v>0</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S12" s="2" t="b">
         <v>0</v>
@@ -10208,7 +10199,7 @@
         <v>240</v>
       </c>
       <c r="AE12" s="2" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="13" spans="1:33" s="3" customFormat="1" ht="400" customHeight="1">
@@ -10249,10 +10240,10 @@
         <v>0</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S13" s="3" t="b">
         <v>0</v>
@@ -10323,22 +10314,22 @@
         <v>0</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="X14" s="2" t="s">
         <v>266</v>
@@ -10353,7 +10344,7 @@
         <v>0</v>
       </c>
       <c r="AB14" s="2" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="AC14" s="2" t="b">
         <v>0</v>
@@ -10362,7 +10353,7 @@
         <v>240</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="15" spans="1:33" s="3" customFormat="1" ht="315" customHeight="1">
@@ -10412,13 +10403,13 @@
         <v>0</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="Q15" s="3" t="b">
         <v>1</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S15" s="3" t="b">
         <v>1</v>
@@ -10471,13 +10462,13 @@
         <v>0</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="Q16" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S16" s="2" t="b">
         <v>0</v>
@@ -10527,25 +10518,25 @@
         <v>0</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S17" s="3" t="b">
         <v>0</v>
       </c>
       <c r="T17" s="3" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="U17" s="3" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="V17" s="3" t="s">
         <v>394</v>
       </c>
       <c r="W17" s="3" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="X17" s="3" t="s">
         <v>266</v>
@@ -10560,7 +10551,7 @@
         <v>0</v>
       </c>
       <c r="AB17" s="3" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AC17" s="3" t="b">
         <v>0</v>
@@ -10619,13 +10610,13 @@
         <v>0</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="Q18" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S18" s="2" t="b">
         <v>0</v>
@@ -10681,13 +10672,13 @@
         <v>0</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="Q19" s="3" t="b">
         <v>1</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S19" s="3" t="b">
         <v>0</v>
@@ -10737,7 +10728,7 @@
         <v>0</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="S20" s="2" t="b">
         <v>1</v>
@@ -10787,37 +10778,37 @@
         <v>1</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S21" s="3" t="b">
         <v>0</v>
       </c>
       <c r="U21" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="V21" s="3" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W21" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="X21" s="3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="Y21" s="3" t="s">
         <v>228</v>
       </c>
       <c r="Z21" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AA21" s="3" t="b">
         <v>0</v>
       </c>
       <c r="AB21" s="3" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="AC21" s="3" t="b">
         <v>0</v>
@@ -10870,25 +10861,25 @@
         <v>0</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="S22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="X22" s="2" t="s">
         <v>266</v>
@@ -10903,16 +10894,16 @@
         <v>0</v>
       </c>
       <c r="AB22" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="AC22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AD22" s="2" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="AE22" s="2" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="23" spans="1:31" s="3" customFormat="1" ht="90" customHeight="1">
@@ -10956,22 +10947,22 @@
         <v>0</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S23" s="3" t="b">
         <v>0</v>
       </c>
       <c r="U23" s="3" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="V23" s="3" t="s">
         <v>400</v>
       </c>
       <c r="W23" s="3" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="X23" s="3" t="s">
         <v>266</v>
@@ -10986,7 +10977,7 @@
         <v>0</v>
       </c>
       <c r="AB23" s="3" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="AC23" s="3" t="b">
         <v>0</v>
@@ -11045,13 +11036,13 @@
         <v>0</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="Q24" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S24" s="2" t="b">
         <v>0</v>
@@ -11101,10 +11092,10 @@
         <v>0</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="R25" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="S25" s="3" t="b">
         <v>0</v>
@@ -11193,13 +11184,13 @@
         <v>0</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="Q26" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S26" s="2" t="b">
         <v>0</v>
@@ -11255,13 +11246,13 @@
         <v>0</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Q27" s="3" t="b">
         <v>1</v>
       </c>
       <c r="R27" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S27" s="3" t="b">
         <v>1</v>
@@ -11308,7 +11299,7 @@
         <v>177</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>490</v>
+        <v>180</v>
       </c>
       <c r="N28" s="2" t="b">
         <v>0</v>
@@ -11317,13 +11308,13 @@
         <v>0</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Q28" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S28" s="2" t="b">
         <v>0</v>
@@ -11373,25 +11364,25 @@
         <v>0</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="R29" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S29" s="3" t="b">
         <v>0</v>
       </c>
       <c r="T29" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="U29" s="3" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="V29" s="3" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="W29" s="3" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="X29" s="3" t="s">
         <v>266</v>
@@ -11406,13 +11397,13 @@
         <v>0</v>
       </c>
       <c r="AB29" s="3" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="AC29" s="3" t="b">
         <v>0</v>
       </c>
       <c r="AD29" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="AE29" s="3" t="s">
         <v>240</v>
@@ -11456,10 +11447,10 @@
         <v>0</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="R30" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="S30" s="2" t="b">
         <v>0</v>
@@ -11527,22 +11518,22 @@
         <v>0</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="R31" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="S31" s="3" t="b">
         <v>0</v>
       </c>
       <c r="U31" s="3" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="V31" s="3" t="s">
         <v>457</v>
       </c>
       <c r="W31" s="3" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="X31" s="3" t="s">
         <v>266</v>
@@ -11557,16 +11548,16 @@
         <v>0</v>
       </c>
       <c r="AB31" s="3" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="AC31" s="3" t="b">
         <v>0</v>
       </c>
       <c r="AD31" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="AE31" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="32" spans="1:31" s="2" customFormat="1" ht="315" customHeight="1">
@@ -11610,31 +11601,31 @@
         <v>0</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="S32" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T32" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="U32" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="V32" s="2" t="s">
         <v>409</v>
       </c>
       <c r="W32" s="2" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="X32" s="2" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="Y32" s="2" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="Z32" s="2" t="s">
         <v>174</v>
@@ -11643,7 +11634,7 @@
         <v>0</v>
       </c>
       <c r="AB32" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="AC32" s="2" t="b">
         <v>0</v>
@@ -11690,7 +11681,7 @@
         <v>177</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="N33" s="3" t="b">
         <v>0</v>
@@ -11699,13 +11690,13 @@
         <v>0</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="Q33" s="3" t="b">
         <v>1</v>
       </c>
       <c r="R33" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S33" s="3" t="b">
         <v>0</v>
@@ -11755,10 +11746,10 @@
         <v>0</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S34" s="2" t="b">
         <v>0</v>
@@ -11785,7 +11776,7 @@
         <v>240</v>
       </c>
       <c r="AE34" s="2" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="35" spans="1:33" s="3" customFormat="1" ht="315" customHeight="1">
@@ -11826,7 +11817,7 @@
         <v>177</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="N35" s="3" t="b">
         <v>0</v>
@@ -11835,13 +11826,13 @@
         <v>0</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="Q35" s="3" t="b">
         <v>1</v>
       </c>
       <c r="R35" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S35" s="3" t="b">
         <v>1</v>
@@ -11891,22 +11882,22 @@
         <v>0</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S36" s="2" t="b">
         <v>0</v>
       </c>
       <c r="U36" s="2" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="V36" s="2" t="s">
         <v>457</v>
       </c>
       <c r="W36" s="2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="X36" s="2" t="s">
         <v>266</v>
@@ -11921,7 +11912,7 @@
         <v>0</v>
       </c>
       <c r="AB36" s="2" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="AC36" s="2" t="b">
         <v>0</v>
@@ -11974,10 +11965,10 @@
         <v>0</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="R37" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="S37" s="3" t="b">
         <v>0</v>
@@ -12063,13 +12054,13 @@
         <v>0</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="Q38" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S38" s="2" t="b">
         <v>1</v>
@@ -12125,13 +12116,13 @@
         <v>0</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="Q39" s="3" t="b">
         <v>1</v>
       </c>
       <c r="R39" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S39" s="3" t="b">
         <v>1</v>
@@ -12181,25 +12172,25 @@
         <v>0</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="S40" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T40" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="U40" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="V40" s="2" t="s">
         <v>416</v>
       </c>
       <c r="W40" s="2" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="X40" s="2" t="s">
         <v>266</v>
@@ -12214,7 +12205,7 @@
         <v>0</v>
       </c>
       <c r="AB40" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="AC40" s="2" t="b">
         <v>0</v>
@@ -12264,7 +12255,7 @@
         <v>177</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="N41" s="3" t="b">
         <v>0</v>
@@ -12273,13 +12264,13 @@
         <v>0</v>
       </c>
       <c r="P41" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="Q41" s="3" t="b">
         <v>1</v>
       </c>
       <c r="R41" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S41" s="3" t="b">
         <v>1</v>
@@ -12326,10 +12317,10 @@
         <v>0</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="R42" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S42" s="2" t="b">
         <v>0</v>
@@ -12391,7 +12382,7 @@
         <v>177</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="N43" s="3" t="b">
         <v>0</v>
@@ -12400,25 +12391,25 @@
         <v>0</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="R43" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="S43" s="3" t="b">
         <v>0</v>
       </c>
       <c r="T43" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="U43" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="V43" s="3" t="s">
         <v>216</v>
       </c>
       <c r="W43" s="3" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="X43" s="3" t="s">
         <v>264</v>
@@ -12433,7 +12424,7 @@
         <v>0</v>
       </c>
       <c r="AB43" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="AC43" s="3" t="b">
         <v>1</v>
@@ -12483,16 +12474,16 @@
         <v>0</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="R44" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="S44" s="2" t="b">
         <v>0</v>
       </c>
       <c r="V44" s="2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="X44" s="2" t="s">
         <v>266</v>
@@ -12557,37 +12548,37 @@
         <v>1</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="R45" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S45" s="3" t="b">
         <v>0</v>
       </c>
       <c r="U45" s="3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="V45" s="3" t="s">
         <v>421</v>
       </c>
       <c r="W45" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="X45" s="3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="Y45" s="3" t="s">
         <v>228</v>
       </c>
       <c r="Z45" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AA45" s="3" t="b">
         <v>0</v>
       </c>
       <c r="AB45" s="3" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="AC45" s="3" t="b">
         <v>0</v>
@@ -12646,13 +12637,13 @@
         <v>0</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="Q46" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R46" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S46" s="2" t="b">
         <v>1</v>
@@ -12702,37 +12693,37 @@
         <v>1</v>
       </c>
       <c r="P47" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="R47" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S47" s="3" t="b">
         <v>0</v>
       </c>
       <c r="U47" s="3" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="V47" s="3" t="s">
         <v>423</v>
       </c>
       <c r="W47" s="3" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="X47" s="3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="Y47" s="3" t="s">
         <v>228</v>
       </c>
       <c r="Z47" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AA47" s="3" t="b">
         <v>0</v>
       </c>
       <c r="AB47" s="3" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="AC47" s="3" t="b">
         <v>0</v>
@@ -12791,13 +12782,13 @@
         <v>0</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="Q48" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R48" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S48" s="2" t="b">
         <v>0</v>
@@ -12844,40 +12835,40 @@
         <v>0</v>
       </c>
       <c r="P49" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="R49" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S49" s="3" t="b">
         <v>0</v>
       </c>
       <c r="T49" s="3" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="U49" s="3" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="V49" s="3" t="s">
         <v>425</v>
       </c>
       <c r="W49" s="3" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="X49" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="Y49" s="3" t="s">
         <v>228</v>
       </c>
       <c r="Z49" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AA49" s="3" t="b">
         <v>0</v>
       </c>
       <c r="AB49" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AC49" s="3" t="b">
         <v>1</v>
@@ -12886,7 +12877,7 @@
         <v>240</v>
       </c>
       <c r="AE49" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="50" spans="1:33" s="2" customFormat="1" ht="90" customHeight="1">
@@ -12933,7 +12924,7 @@
         <v>194</v>
       </c>
       <c r="R50" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S50" s="2" t="b">
         <v>0</v>
@@ -13025,13 +13016,13 @@
         <v>0</v>
       </c>
       <c r="P51" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="Q51" s="3" t="b">
         <v>1</v>
       </c>
       <c r="R51" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S51" s="3" t="b">
         <v>0</v>
@@ -13081,16 +13072,16 @@
         <v>0</v>
       </c>
       <c r="P52" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="R52" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="S52" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T52" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="U52" s="2" t="s">
         <v>234</v>
@@ -13123,7 +13114,7 @@
         <v>240</v>
       </c>
       <c r="AE52" s="2" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="53" spans="1:33" s="3" customFormat="1" ht="315" customHeight="1">
@@ -13167,13 +13158,13 @@
         <v>0</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="Q53" s="3" t="b">
         <v>0</v>
       </c>
       <c r="R53" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S53" s="3" t="b">
         <v>0</v>
@@ -13226,37 +13217,37 @@
         <v>1</v>
       </c>
       <c r="P54" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="R54" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S54" s="2" t="b">
         <v>0</v>
       </c>
       <c r="U54" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="V54" s="2" t="s">
         <v>429</v>
       </c>
       <c r="W54" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="X54" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="Y54" s="2" t="s">
         <v>228</v>
       </c>
       <c r="Z54" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AA54" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AB54" s="2" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="AC54" s="2" t="b">
         <v>0</v>
@@ -13306,10 +13297,10 @@
         <v>0</v>
       </c>
       <c r="P55" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="R55" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S55" s="3" t="b">
         <v>0</v>
@@ -13377,7 +13368,7 @@
         <v>177</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="N56" s="2" t="b">
         <v>0</v>
@@ -13386,13 +13377,13 @@
         <v>0</v>
       </c>
       <c r="P56" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="Q56" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S56" s="2" t="b">
         <v>1</v>
@@ -13433,7 +13424,7 @@
         <v>177</v>
       </c>
       <c r="M57" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="N57" s="3" t="b">
         <v>0</v>
@@ -13442,28 +13433,28 @@
         <v>0</v>
       </c>
       <c r="P57" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="R57" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S57" s="3" t="b">
         <v>0</v>
       </c>
       <c r="T57" s="3" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="U57" s="3" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="V57" s="3" t="s">
         <v>432</v>
       </c>
       <c r="W57" s="3" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="X57" s="3" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="Y57" s="3" t="s">
         <v>228</v>
@@ -13475,7 +13466,7 @@
         <v>0</v>
       </c>
       <c r="AB57" s="3" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="AC57" s="3" t="b">
         <v>0</v>
@@ -13528,22 +13519,22 @@
         <v>0</v>
       </c>
       <c r="P58" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="R58" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S58" s="2" t="b">
         <v>0</v>
       </c>
       <c r="U58" s="2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="V58" s="2" t="s">
         <v>400</v>
       </c>
       <c r="W58" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="X58" s="2" t="s">
         <v>266</v>
@@ -13558,7 +13549,7 @@
         <v>0</v>
       </c>
       <c r="AB58" s="2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="AC58" s="2" t="b">
         <v>0</v>
@@ -13608,10 +13599,10 @@
         <v>0</v>
       </c>
       <c r="P59" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="R59" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S59" s="3" t="b">
         <v>0</v>
@@ -13682,37 +13673,37 @@
         <v>1</v>
       </c>
       <c r="P60" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="R60" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S60" s="2" t="b">
         <v>0</v>
       </c>
       <c r="U60" s="2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="V60" s="2" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="W60" s="2" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="X60" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="Y60" s="2" t="s">
         <v>228</v>
       </c>
       <c r="Z60" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AA60" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AB60" s="2" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="AC60" s="2" t="b">
         <v>0</v>
@@ -13768,13 +13759,13 @@
         <v>0</v>
       </c>
       <c r="P61" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="Q61" s="3" t="b">
         <v>1</v>
       </c>
       <c r="R61" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S61" s="3" t="b">
         <v>0</v>
@@ -13815,7 +13806,7 @@
         <v>177</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="N62" s="2" t="b">
         <v>0</v>
@@ -13824,25 +13815,25 @@
         <v>0</v>
       </c>
       <c r="P62" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="R62" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S62" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T62" s="2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="U62" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V62" s="2" t="s">
         <v>437</v>
       </c>
       <c r="W62" s="2" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="X62" s="2" t="s">
         <v>266</v>
@@ -13857,7 +13848,7 @@
         <v>0</v>
       </c>
       <c r="AB62" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="AC62" s="2" t="b">
         <v>0</v>
@@ -13913,7 +13904,7 @@
         <v>0</v>
       </c>
       <c r="R63" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="S63" s="3" t="b">
         <v>1</v>
@@ -13954,7 +13945,7 @@
         <v>177</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="N64" s="2" t="b">
         <v>0</v>
@@ -13963,25 +13954,25 @@
         <v>0</v>
       </c>
       <c r="P64" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="R64" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S64" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T64" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="U64" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="V64" s="2" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="W64" s="2" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="X64" s="2" t="s">
         <v>266</v>
@@ -13996,7 +13987,7 @@
         <v>0</v>
       </c>
       <c r="AB64" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="AC64" s="2" t="b">
         <v>0</v>
@@ -14005,7 +13996,7 @@
         <v>240</v>
       </c>
       <c r="AE64" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="65" spans="1:33" s="3" customFormat="1" ht="105" customHeight="1">
@@ -14040,7 +14031,7 @@
         <v>177</v>
       </c>
       <c r="M65" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="N65" s="3" t="b">
         <v>0</v>
@@ -14049,22 +14040,22 @@
         <v>0</v>
       </c>
       <c r="P65" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="R65" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S65" s="3" t="b">
         <v>0</v>
       </c>
       <c r="U65" s="3" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="V65" s="3" t="s">
         <v>440</v>
       </c>
       <c r="W65" s="3" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="X65" s="3" t="s">
         <v>266</v>
@@ -14079,7 +14070,7 @@
         <v>0</v>
       </c>
       <c r="AB65" s="3" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="AC65" s="3" t="b">
         <v>0</v>
@@ -14126,7 +14117,7 @@
         <v>177</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="N66" s="2" t="b">
         <v>0</v>
@@ -14135,13 +14126,13 @@
         <v>0</v>
       </c>
       <c r="P66" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="Q66" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R66" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S66" s="2" t="b">
         <v>0</v>
@@ -14185,7 +14176,7 @@
         <v>177</v>
       </c>
       <c r="M67" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="N67" s="3" t="b">
         <v>0</v>
@@ -14194,40 +14185,40 @@
         <v>0</v>
       </c>
       <c r="P67" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="R67" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S67" s="3" t="b">
         <v>0</v>
       </c>
       <c r="T67" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="U67" s="3" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="V67" s="3" t="s">
         <v>442</v>
       </c>
       <c r="W67" s="3" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="X67" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="Y67" s="3" t="s">
         <v>228</v>
       </c>
       <c r="Z67" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AA67" s="3" t="b">
         <v>0</v>
       </c>
       <c r="AB67" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="AC67" s="3" t="b">
         <v>1</v>
@@ -14236,10 +14227,10 @@
         <v>240</v>
       </c>
       <c r="AE67" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="AF67" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="68" spans="1:33" s="2" customFormat="1" ht="400" customHeight="1">
@@ -14286,13 +14277,13 @@
         <v>0</v>
       </c>
       <c r="P68" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="Q68" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R68" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S68" s="2" t="b">
         <v>0</v>
@@ -14351,13 +14342,13 @@
         <v>0</v>
       </c>
       <c r="P69" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="Q69" s="3" t="b">
         <v>1</v>
       </c>
       <c r="R69" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S69" s="3" t="b">
         <v>0</v>
@@ -14407,22 +14398,22 @@
         <v>0</v>
       </c>
       <c r="P70" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="R70" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="S70" s="2" t="b">
         <v>0</v>
       </c>
       <c r="U70" s="2" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="V70" s="2" t="s">
         <v>445</v>
       </c>
       <c r="W70" s="2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="X70" s="2" t="s">
         <v>268</v>
@@ -14437,7 +14428,7 @@
         <v>0</v>
       </c>
       <c r="AB70" s="2" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="AC70" s="2" t="b">
         <v>0</v>
@@ -14490,10 +14481,10 @@
         <v>0</v>
       </c>
       <c r="P71" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="R71" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="S71" s="3" t="b">
         <v>0</v>
@@ -14529,7 +14520,7 @@
         <v>240</v>
       </c>
       <c r="AE71" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="72" spans="1:33" s="2" customFormat="1" ht="400" customHeight="1">
@@ -14570,10 +14561,10 @@
         <v>0</v>
       </c>
       <c r="P72" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="R72" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="S72" s="2" t="b">
         <v>0</v>
@@ -14644,37 +14635,37 @@
         <v>1</v>
       </c>
       <c r="P73" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="R73" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S73" s="3" t="b">
         <v>0</v>
       </c>
       <c r="U73" s="3" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="V73" s="3" t="s">
         <v>447</v>
       </c>
       <c r="W73" s="3" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="X73" s="3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="Y73" s="3" t="s">
         <v>228</v>
       </c>
       <c r="Z73" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AA73" s="3" t="b">
         <v>0</v>
       </c>
       <c r="AB73" s="3" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="AC73" s="3" t="b">
         <v>1</v>
@@ -14727,22 +14718,22 @@
         <v>0</v>
       </c>
       <c r="P74" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="R74" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S74" s="2" t="b">
         <v>0</v>
       </c>
       <c r="U74" s="2" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="V74" s="2" t="s">
         <v>448</v>
       </c>
       <c r="W74" s="2" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="X74" s="2" t="s">
         <v>266</v>
@@ -14757,7 +14748,7 @@
         <v>0</v>
       </c>
       <c r="AB74" s="2" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="AC74" s="2" t="b">
         <v>0</v>
@@ -14810,25 +14801,25 @@
         <v>0</v>
       </c>
       <c r="P75" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="R75" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S75" s="3" t="b">
         <v>0</v>
       </c>
       <c r="T75" s="3" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="U75" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="V75" s="3" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="W75" s="3" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="X75" s="3" t="s">
         <v>266</v>
@@ -14843,7 +14834,7 @@
         <v>0</v>
       </c>
       <c r="AB75" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="AC75" s="3" t="b">
         <v>0</v>
@@ -14852,7 +14843,7 @@
         <v>240</v>
       </c>
       <c r="AE75" s="3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="76" spans="1:33" s="2" customFormat="1" ht="400" customHeight="1">
@@ -14893,10 +14884,10 @@
         <v>0</v>
       </c>
       <c r="P76" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="R76" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S76" s="2" t="b">
         <v>0</v>
@@ -14967,40 +14958,40 @@
         <v>0</v>
       </c>
       <c r="P77" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="R77" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S77" s="3" t="b">
         <v>0</v>
       </c>
       <c r="T77" s="3" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="U77" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="V77" s="3" t="s">
         <v>451</v>
       </c>
       <c r="W77" s="3" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="X77" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="Y77" s="3" t="s">
         <v>228</v>
       </c>
       <c r="Z77" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AA77" s="3" t="b">
         <v>0</v>
       </c>
       <c r="AB77" s="3" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="AC77" s="3" t="b">
         <v>1</v>
@@ -15009,7 +15000,7 @@
         <v>240</v>
       </c>
       <c r="AE77" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="78" spans="1:33" s="2" customFormat="1" ht="400" customHeight="1">
@@ -15053,37 +15044,37 @@
         <v>1</v>
       </c>
       <c r="P78" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="R78" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="S78" s="2" t="b">
         <v>0</v>
       </c>
       <c r="U78" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="V78" s="2" t="s">
         <v>452</v>
       </c>
       <c r="W78" s="2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="X78" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="Y78" s="2" t="s">
         <v>228</v>
       </c>
       <c r="Z78" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AA78" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AB78" s="2" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="AC78" s="2" t="b">
         <v>0</v>
@@ -15136,25 +15127,25 @@
         <v>0</v>
       </c>
       <c r="P79" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="R79" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="S79" s="3" t="b">
         <v>0</v>
       </c>
       <c r="T79" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="U79" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="V79" s="3" t="s">
         <v>216</v>
       </c>
       <c r="W79" s="3" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="X79" s="3" t="s">
         <v>264</v>
@@ -15169,7 +15160,7 @@
         <v>0</v>
       </c>
       <c r="AB79" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="AC79" s="3" t="b">
         <v>1</v>
@@ -15178,7 +15169,7 @@
         <v>240</v>
       </c>
       <c r="AE79" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="80" spans="1:33" s="2" customFormat="1" ht="300" customHeight="1">
@@ -15219,10 +15210,10 @@
         <v>0</v>
       </c>
       <c r="P80" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="R80" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S80" s="2" t="b">
         <v>0</v>
@@ -15284,7 +15275,7 @@
         <v>177</v>
       </c>
       <c r="M81" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="N81" s="3" t="b">
         <v>0</v>
@@ -15293,25 +15284,25 @@
         <v>0</v>
       </c>
       <c r="P81" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="R81" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S81" s="3" t="b">
         <v>0</v>
       </c>
       <c r="T81" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="U81" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="V81" s="3" t="s">
         <v>216</v>
       </c>
       <c r="W81" s="3" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="X81" s="3" t="s">
         <v>266</v>
@@ -15326,7 +15317,7 @@
         <v>0</v>
       </c>
       <c r="AB81" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="AC81" s="3" t="b">
         <v>0</v>
@@ -15379,37 +15370,37 @@
         <v>0</v>
       </c>
       <c r="P82" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="R82" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S82" s="2" t="b">
         <v>0</v>
       </c>
       <c r="U82" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="V82" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="W82" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="X82" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="Y82" s="2" t="s">
         <v>228</v>
       </c>
       <c r="Z82" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AA82" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AB82" s="2" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="AC82" s="2" t="b">
         <v>1</v>
@@ -15462,22 +15453,22 @@
         <v>0</v>
       </c>
       <c r="P83" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="R83" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="S83" s="3" t="b">
         <v>0</v>
       </c>
       <c r="U83" s="3" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="V83" s="3" t="s">
         <v>457</v>
       </c>
       <c r="W83" s="3" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="X83" s="3" t="s">
         <v>266</v>
@@ -15492,13 +15483,13 @@
         <v>0</v>
       </c>
       <c r="AB83" s="3" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="AC83" s="3" t="b">
         <v>0</v>
       </c>
       <c r="AD83" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="AE83" s="3" t="s">
         <v>240</v>
@@ -15542,10 +15533,10 @@
         <v>0</v>
       </c>
       <c r="P84" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="R84" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S84" s="2" t="b">
         <v>0</v>
@@ -15569,7 +15560,7 @@
         <v>231</v>
       </c>
       <c r="AD84" s="2" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="AE84" s="2" t="s">
         <v>240</v>
@@ -15613,10 +15604,10 @@
         <v>0</v>
       </c>
       <c r="P85" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="R85" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="S85" s="3" t="b">
         <v>0</v>
@@ -15684,25 +15675,25 @@
         <v>0</v>
       </c>
       <c r="P86" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="R86" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="S86" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T86" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="U86" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="V86" s="2" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="W86" s="2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="X86" s="2" t="s">
         <v>266</v>
@@ -15717,7 +15708,7 @@
         <v>0</v>
       </c>
       <c r="AB86" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="AC86" s="2" t="b">
         <v>0</v>
@@ -15776,13 +15767,13 @@
         <v>0</v>
       </c>
       <c r="P87" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="Q87" s="3" t="b">
         <v>1</v>
       </c>
       <c r="R87" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S87" s="3" t="b">
         <v>1</v>
@@ -15832,37 +15823,37 @@
         <v>1</v>
       </c>
       <c r="P88" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="R88" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S88" s="2" t="b">
         <v>0</v>
       </c>
       <c r="U88" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="V88" s="2" t="s">
         <v>462</v>
       </c>
       <c r="W88" s="2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="X88" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="Y88" s="2" t="s">
         <v>228</v>
       </c>
       <c r="Z88" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AA88" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AB88" s="2" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="AC88" s="2" t="b">
         <v>1</v>
@@ -15915,25 +15906,25 @@
         <v>0</v>
       </c>
       <c r="P89" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="R89" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S89" s="3" t="b">
         <v>0</v>
       </c>
       <c r="T89" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="U89" s="3" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="V89" s="3" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="W89" s="3" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="X89" s="3" t="s">
         <v>266</v>
@@ -15948,7 +15939,7 @@
         <v>0</v>
       </c>
       <c r="AB89" s="3" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="AC89" s="3" t="b">
         <v>0</v>
@@ -16001,25 +15992,25 @@
         <v>0</v>
       </c>
       <c r="P90" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="R90" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S90" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T90" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="U90" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="V90" s="2" t="s">
         <v>464</v>
       </c>
       <c r="W90" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="X90" s="2" t="s">
         <v>266</v>
@@ -16034,7 +16025,7 @@
         <v>0</v>
       </c>
       <c r="AB90" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="AC90" s="2" t="b">
         <v>0</v>
@@ -16087,40 +16078,40 @@
         <v>0</v>
       </c>
       <c r="P91" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="R91" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S91" s="3" t="b">
         <v>0</v>
       </c>
       <c r="T91" s="3" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="U91" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="V91" s="3" t="s">
         <v>465</v>
       </c>
       <c r="W91" s="3" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="X91" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="Y91" s="3" t="s">
         <v>228</v>
       </c>
       <c r="Z91" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AA91" s="3" t="b">
         <v>0</v>
       </c>
       <c r="AB91" s="3" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="AC91" s="3" t="b">
         <v>1</v>
@@ -16129,7 +16120,7 @@
         <v>240</v>
       </c>
       <c r="AE91" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="92" spans="1:31" s="2" customFormat="1" ht="390" customHeight="1">
@@ -16173,37 +16164,37 @@
         <v>1</v>
       </c>
       <c r="P92" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="R92" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S92" s="2" t="b">
         <v>0</v>
       </c>
       <c r="U92" s="2" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="V92" s="2" t="s">
         <v>466</v>
       </c>
       <c r="W92" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="X92" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="Y92" s="2" t="s">
         <v>228</v>
       </c>
       <c r="Z92" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AA92" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AB92" s="2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="AC92" s="2" t="b">
         <v>0</v>
@@ -16256,10 +16247,10 @@
         <v>0</v>
       </c>
       <c r="P93" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="R93" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S93" s="3" t="b">
         <v>0</v>
@@ -16339,40 +16330,40 @@
         <v>0</v>
       </c>
       <c r="P94" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="R94" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S94" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T94" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="U94" s="2" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="V94" s="2" t="s">
         <v>467</v>
       </c>
       <c r="W94" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="X94" s="2" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="Y94" s="2" t="s">
         <v>228</v>
       </c>
       <c r="Z94" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AA94" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AB94" s="2" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="AC94" s="2" t="b">
         <v>1</v>
@@ -16381,7 +16372,7 @@
         <v>240</v>
       </c>
       <c r="AE94" s="2" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="95" spans="1:31" s="3" customFormat="1" ht="400" customHeight="1">
@@ -16425,25 +16416,25 @@
         <v>0</v>
       </c>
       <c r="P95" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="R95" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S95" s="3" t="b">
         <v>0</v>
       </c>
       <c r="T95" s="3" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="U95" s="3" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="V95" s="3" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="W95" s="3" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="X95" s="3" t="s">
         <v>266</v>
@@ -16458,13 +16449,13 @@
         <v>0</v>
       </c>
       <c r="AB95" s="3" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="AC95" s="3" t="b">
         <v>0</v>
       </c>
       <c r="AD95" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="AE95" s="3" t="s">
         <v>240</v>
@@ -16511,25 +16502,25 @@
         <v>0</v>
       </c>
       <c r="P96" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="R96" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S96" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T96" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="U96" s="2" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="V96" s="2" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="W96" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="X96" s="2" t="s">
         <v>266</v>
@@ -16544,7 +16535,7 @@
         <v>0</v>
       </c>
       <c r="AB96" s="2" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="AC96" s="2" t="b">
         <v>0</v>
@@ -16597,25 +16588,25 @@
         <v>0</v>
       </c>
       <c r="P97" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="R97" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S97" s="3" t="b">
         <v>0</v>
       </c>
       <c r="T97" s="3" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="U97" s="3" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="V97" s="3" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="W97" s="3" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="X97" s="3" t="s">
         <v>266</v>
@@ -16630,7 +16621,7 @@
         <v>0</v>
       </c>
       <c r="AB97" s="3" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="AC97" s="3" t="b">
         <v>0</v>
@@ -16683,25 +16674,25 @@
         <v>0</v>
       </c>
       <c r="P98" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="R98" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="S98" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T98" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="U98" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="V98" s="2" t="s">
         <v>216</v>
       </c>
       <c r="W98" s="2" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="X98" s="2" t="s">
         <v>264</v>
@@ -16716,7 +16707,7 @@
         <v>0</v>
       </c>
       <c r="AB98" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="AC98" s="2" t="b">
         <v>1</v>
@@ -16757,7 +16748,7 @@
         <v>177</v>
       </c>
       <c r="M99" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N99" s="3" t="b">
         <v>0</v>
@@ -16766,16 +16757,16 @@
         <v>0</v>
       </c>
       <c r="P99" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="R99" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S99" s="3" t="b">
         <v>0</v>
       </c>
       <c r="T99" s="3" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="V99" s="3" t="s">
         <v>472</v>
@@ -16834,7 +16825,7 @@
         <v>177</v>
       </c>
       <c r="M100" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="N100" s="2" t="b">
         <v>0</v>
@@ -16843,25 +16834,25 @@
         <v>0</v>
       </c>
       <c r="P100" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="R100" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S100" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T100" s="2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="U100" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="V100" s="2" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="W100" s="2" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="X100" s="2" t="s">
         <v>266</v>
@@ -16876,13 +16867,13 @@
         <v>0</v>
       </c>
       <c r="AB100" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="AC100" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AD100" s="2" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="AE100" s="2" t="s">
         <v>240</v>
@@ -16935,13 +16926,13 @@
         <v>0</v>
       </c>
       <c r="P101" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="Q101" s="3" t="b">
         <v>1</v>
       </c>
       <c r="R101" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S101" s="3" t="b">
         <v>1</v>
@@ -16991,22 +16982,22 @@
         <v>0</v>
       </c>
       <c r="P102" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="R102" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S102" s="2" t="b">
         <v>0</v>
       </c>
       <c r="U102" s="2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="V102" s="2" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="W102" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="X102" s="2" t="s">
         <v>266</v>
@@ -17021,7 +17012,7 @@
         <v>0</v>
       </c>
       <c r="AB102" s="2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="AC102" s="2" t="b">
         <v>0</v>
@@ -17030,7 +17021,7 @@
         <v>240</v>
       </c>
       <c r="AE102" s="2" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="103" spans="1:31" s="3" customFormat="1" ht="390" customHeight="1">
@@ -17074,40 +17065,40 @@
         <v>0</v>
       </c>
       <c r="P103" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="R103" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S103" s="3" t="b">
         <v>0</v>
       </c>
       <c r="T103" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="U103" s="3" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="V103" s="3" t="s">
         <v>476</v>
       </c>
       <c r="W103" s="3" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="X103" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="Y103" s="3" t="s">
         <v>228</v>
       </c>
       <c r="Z103" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AA103" s="3" t="b">
         <v>0</v>
       </c>
       <c r="AB103" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="AC103" s="3" t="b">
         <v>1</v>
@@ -17116,7 +17107,7 @@
         <v>240</v>
       </c>
       <c r="AE103" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="104" spans="1:31" s="2" customFormat="1" ht="90" customHeight="1">
@@ -17160,25 +17151,25 @@
         <v>0</v>
       </c>
       <c r="P104" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="R104" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S104" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T104" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="U104" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="V104" s="2" t="s">
         <v>477</v>
       </c>
       <c r="W104" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="X104" s="2" t="s">
         <v>266</v>
@@ -17193,7 +17184,7 @@
         <v>0</v>
       </c>
       <c r="AB104" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="AC104" s="2" t="b">
         <v>0</v>
@@ -17246,37 +17237,37 @@
         <v>1</v>
       </c>
       <c r="P105" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="R105" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S105" s="3" t="b">
         <v>0</v>
       </c>
       <c r="U105" s="3" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="V105" s="3" t="s">
         <v>478</v>
       </c>
       <c r="W105" s="3" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="X105" s="3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="Y105" s="3" t="s">
         <v>228</v>
       </c>
       <c r="Z105" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AA105" s="3" t="b">
         <v>0</v>
       </c>
       <c r="AB105" s="3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="AC105" s="3" t="b">
         <v>0</v>

</xml_diff>